<commit_message>
Solicitud gráfica recursos 50 y 140
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion01/SolicitudGrafica MA_11_01_CO_REC50f6.xlsx
+++ b/fuentes/contenidos/grado11/guion01/SolicitudGrafica MA_11_01_CO_REC50f6.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pahola\Desktop\Aula- Planeta\MA_11_01-CO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8955" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9825" windowHeight="3570" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitud gráfica" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="206">
   <si>
     <t>Fecha:</t>
   </si>
@@ -608,64 +608,45 @@
     <t>Ilustración</t>
   </si>
   <si>
-    <t>http://www.shutterstock.com/cat.mhtml?lang=es&amp;language=es&amp;ref_site=photo&amp;search_source=search_form&amp;version=llv1&amp;anyorall=all&amp;safesearch=1&amp;use_local_boost=1&amp;autocomplete_id=&amp;searchterm=numeros%20irracionales&amp;show_color_wheel=1&amp;orient=&amp;commercial_ok=&amp;media_type=images&amp;search_cat=&amp;searchtermx=&amp;photographer_name=&amp;people_gender=&amp;people_age=&amp;people_ethnicity=&amp;people_number=&amp;color=&amp;page=1&amp;inline=54319891</t>
-  </si>
-  <si>
-    <t>http://www.shutterstock.com/cat.mhtml?lang=es&amp;language=es&amp;ref_site=photo&amp;search_source=search_form&amp;version=llv1&amp;anyorall=all&amp;safesearch=1&amp;use_local_boost=1&amp;autocomplete_id=&amp;search_tracking_id=qX0Xhf95jmBSsyEjNavreQ&amp;searchterm=historia%20y%20matematicas&amp;show_color_wheel=1&amp;orient=&amp;commercial_ok=&amp;media_type=images&amp;search_cat=&amp;searchtermx=&amp;photographer_name=&amp;people_gender=&amp;people_age=&amp;people_ethnicity=&amp;people_number=&amp;color=&amp;page=1&amp;inline=329134130</t>
-  </si>
-  <si>
-    <t>http://www.shutterstock.com/similar-336975836/stock-vector-square-root-equation-icon-vector-image-can-also-be-used-for-education-and-science-suitable-for.html?page=1&amp;inline=407568826</t>
-  </si>
-  <si>
-    <t>http://www.shutterstock.com/cat.mhtml?lang=es&amp;language=es&amp;ref_site=photo&amp;search_source=search_form&amp;version=llv1&amp;anyorall=all&amp;safesearch=1&amp;use_local_boost=1&amp;autocomplete_id=&amp;search_tracking_id=55HwENMlVJi2CV0EnR4JOA&amp;searchterm=operaciones%20matematica&amp;show_color_wheel=1&amp;orient=&amp;commercial_ok=&amp;media_type=images&amp;search_cat=&amp;searchtermx=&amp;photographer_name=&amp;people_gender=&amp;people_age=&amp;people_ethnicity=&amp;people_number=&amp;color=&amp;page=1&amp;inline=116463280</t>
-  </si>
-  <si>
-    <t>http://www.shutterstock.com/cat.mhtml?country_code=CO&amp;safesearch=1&amp;search_language=es&amp;search_type=keyword_search&amp;searchterm=irracional&amp;sort_method=popular&amp;use_local_boost=1&amp;version=llv1&amp;search_source=recent_search_csl&amp;page=1&amp;inline=287681024</t>
-  </si>
-  <si>
     <t>Imagen para boton 3.</t>
   </si>
   <si>
-    <t>Imagen para la primera ficha del botón 1, usar normal y ampliada</t>
-  </si>
-  <si>
-    <t>http://www.shutterstock.com/cat.mhtml?lang=es&amp;language=es&amp;ref_site=photo&amp;search_source=search_form&amp;version=llv1&amp;anyorall=all&amp;safesearch=1&amp;use_local_boost=1&amp;autocomplete_id=&amp;search_tracking_id=HFiX1ZalQgd6MO5MRywQDQ&amp;searchterm=matematicas&amp;show_color_wheel=1&amp;orient=&amp;commercial_ok=&amp;media_type=images&amp;search_cat=&amp;searchtermx=&amp;photographer_name=&amp;people_gender=&amp;people_age=&amp;people_ethnicity=&amp;people_number=&amp;color=&amp;page=1&amp;inline=121813099</t>
-  </si>
-  <si>
     <t>Imagen para la segunda ficha del botón 1, usar normal y ampliada</t>
   </si>
   <si>
-    <t>http://www.shutterstock.com/cat.mhtml?lang=es&amp;language=es&amp;ref_site=photo&amp;search_source=search_form&amp;version=llv1&amp;anyorall=all&amp;safesearch=1&amp;use_local_boost=1&amp;autocomplete_id=&amp;search_tracking_id=REPNaRpe_sVZtA8PqgZPzQ&amp;searchterm=matematicas%20e%20historia&amp;show_color_wheel=1&amp;orient=&amp;commercial_ok=&amp;media_type=images&amp;search_cat=&amp;searchtermx=&amp;photographer_name=&amp;people_gender=&amp;people_age=&amp;people_ethnicity=&amp;people_number=&amp;color=&amp;page=1&amp;inline=329134130</t>
-  </si>
-  <si>
     <t>Imagen para la tercera ficha del botón 1, usar normal y ampliada</t>
   </si>
   <si>
     <t>Imagen para la primera ficha del botón 2, usar normal y ampliada</t>
   </si>
   <si>
-    <t>Usar imagen adjunta en la observación (cuadrado con su diagonal marcada y un lado resaltado, además de estos mismos lados mostrarse al lado del cuadrado, el uso de colores es fundamental) , esá imagen se usa para la ficha dos del boton 2, (imagen 1, normal y ampliada)</t>
-  </si>
-  <si>
-    <t>Usar imagen adjunta en la observación (es importante que la imagen tenga toda la información igual) , esá imagen se usa para la ficha dos del boton 2, (imagen 2, normal y ampliada)</t>
-  </si>
-  <si>
-    <t>Imagen similar a la que aparece en la observación (debe estar el número phi y e), la imagen se usa en la ficha 1 del botón 3 normal y ampliada.</t>
-  </si>
-  <si>
     <t>Pentágono igual al que aparece en la observación ( es importante que tenga toda la información), la imagen se usa en la ficha dos del botón 3. Imagen 1 normal y ampliada.</t>
   </si>
   <si>
     <t>Billete de diez mil pesos con el rectángulo blaco resaltado, la imagen se usa para la ficha 3 del botón 3.</t>
   </si>
   <si>
-    <t>http://www.shutterstock.com/cat.mhtml?lang=es&amp;language=es&amp;ref_site=photo&amp;search_source=search_form&amp;version=llv1&amp;anyorall=all&amp;safesearch=1&amp;use_local_boost=1&amp;autocomplete_id=&amp;search_tracking_id=U6X8VA9C4pPW4GA48oETVw&amp;searchterm=espiral%20de%20oro&amp;show_color_wheel=1&amp;orient=&amp;commercial_ok=&amp;media_type=images&amp;search_cat=&amp;searchtermx=&amp;photographer_name=&amp;people_gender=&amp;people_age=&amp;people_ethnicity=&amp;people_number=&amp;color=&amp;page=1&amp;inline=117359608</t>
-  </si>
-  <si>
     <t>Imagen usada para la ficha 4 del botón 3, normal y ampliada. Usar también como icono de recurso</t>
   </si>
   <si>
     <t>Imagen para ubicar en la ficha del estudiante. Tabla adjunta en la observación</t>
+  </si>
+  <si>
+    <t>Ver descripción</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La imagen se construyó para el rec70. Ajusatrla para rec50, nueva versión del material. Nombrar como imagen 04. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es la imagen MA_11_01_CO_REC30_IMG01. Actualizar nombre y tamaño si es necesario
+</t>
+  </si>
+  <si>
+    <t>Es la imagen MA_11_01_CO_REC30_IMG02. Actualizar nombre y tamaño si es necesario</t>
+  </si>
+  <si>
+    <t>Ver indicación al final del archivo</t>
   </si>
 </sst>
 </file>
@@ -675,7 +656,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -835,6 +816,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1331,7 +1318,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1383,8 +1370,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1607,6 +1595,8 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="51"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1706,7 +1696,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="52">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -1732,6 +1722,7 @@
     <cellStyle name="Hipervínculo" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="51" builtinId="8"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -1811,7 +1802,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" sel="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1828,81 +1819,28 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>196013</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>154781</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>547688</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>215331</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1940718</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>1190626</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>4701985</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1349375</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2" descr="http://brownsharpie.courtneygibbons.org/wp-content/comics/2009-12-07-transcendental.jpg"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect r="8037" b="24334"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="16543294" y="19645312"/>
-          <a:ext cx="1744705" cy="1035845"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>321469</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>11906</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>683419</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>1764506</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Imagen 1"/>
+        <xdr:cNvPr id="7" name="Imagen 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1916,76 +1854,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="16668750" y="16025812"/>
-          <a:ext cx="4291013" cy="1752600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>309563</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>241110</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>1452563</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Imagen 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="16656844" y="17847470"/>
-          <a:ext cx="2193735" cy="1452562"/>
+          <a:off x="14779626" y="6454206"/>
+          <a:ext cx="4154297" cy="1134044"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2038,7 +1908,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2106,7 +1976,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:srcRect l="20958" t="31253" r="44204" b="35540"/>
         <a:stretch/>
       </xdr:blipFill>
@@ -2130,14 +2000,90 @@
       <xdr:rowOff>217714</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>435428</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2943669</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>1354050</xdr:rowOff>
+      <xdr:rowOff>1471084</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20052393" y="14928547"/>
+          <a:ext cx="2671526" cy="1253370"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>238743</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>233796</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>4789714</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>3000898</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13954743" y="28699939"/>
+          <a:ext cx="4550971" cy="2767102"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>484188</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>62661</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3659188</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1612363</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2150,8 +2096,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16641536" y="27010178"/>
-          <a:ext cx="2422071" cy="1136336"/>
+          <a:off x="14716126" y="4460036"/>
+          <a:ext cx="3175000" cy="1549702"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2878,9 +2824,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2890,12 +2836,12 @@
     <col min="3" max="3" width="21.25" style="2" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="17.25" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.25" style="2" customWidth="1"/>
+    <col min="6" max="6" width="33.25" style="2" customWidth="1"/>
     <col min="7" max="7" width="20.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="28.625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="35.375" style="2" customWidth="1"/>
     <col min="9" max="9" width="20.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="34.875" style="15" customWidth="1"/>
-    <col min="11" max="11" width="29.625" style="15" customWidth="1"/>
+    <col min="10" max="10" width="67.875" style="15" customWidth="1"/>
+    <col min="11" max="11" width="70.75" style="15" customWidth="1"/>
     <col min="12" max="12" width="20.375" style="2" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="14.5" style="2" hidden="1" customWidth="1"/>
     <col min="14" max="15" width="10.875" style="2" hidden="1" customWidth="1"/>
@@ -2926,14 +2872,14 @@
       <c r="B2" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="86"/>
-      <c r="F2" s="78" t="s">
+      <c r="D2" s="88"/>
+      <c r="F2" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="79"/>
+      <c r="G2" s="81"/>
       <c r="H2" s="58"/>
       <c r="I2" s="58"/>
       <c r="J2" s="14"/>
@@ -2957,12 +2903,12 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="87">
+      <c r="C3" s="89">
         <v>11</v>
       </c>
-      <c r="D3" s="88"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="81"/>
+      <c r="D3" s="90"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="83"/>
       <c r="H3" s="58"/>
       <c r="I3" s="38"/>
       <c r="J3" s="14"/>
@@ -2986,10 +2932,10 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="D4" s="88"/>
+      <c r="D4" s="90"/>
       <c r="E4" s="5"/>
       <c r="F4" s="37" t="s">
         <v>55</v>
@@ -3018,10 +2964,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="89" t="s">
+      <c r="C5" s="91" t="s">
         <v>188</v>
       </c>
-      <c r="D5" s="90"/>
+      <c r="D5" s="92"/>
       <c r="E5" s="5"/>
       <c r="F5" s="37" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -3105,12 +3051,12 @@
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="82" t="s">
+      <c r="F8" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="84"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="85"/>
+      <c r="I8" s="86"/>
       <c r="J8" s="16"/>
       <c r="K8" s="11"/>
       <c r="M8" s="2" t="str">
@@ -3166,13 +3112,13 @@
         <v>M10B</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="11" customFormat="1" ht="297" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
       </c>
-      <c r="B10" s="62" t="s">
-        <v>194</v>
+      <c r="B10" s="62">
+        <v>329134130</v>
       </c>
       <c r="C10" s="20" t="str">
         <f t="shared" ref="C10:C41" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
@@ -3214,8 +3160,8 @@
         <f t="shared" ref="A11:A18" si="3">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
       </c>
-      <c r="B11" s="62" t="s">
-        <v>195</v>
+      <c r="B11" s="78">
+        <v>20092879</v>
       </c>
       <c r="C11" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3252,13 +3198,13 @@
         <v>M101</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG03</v>
       </c>
-      <c r="B12" s="62" t="s">
-        <v>197</v>
+      <c r="B12" s="78">
+        <v>77507800</v>
       </c>
       <c r="C12" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3287,7 +3233,7 @@
         <v/>
       </c>
       <c r="J12" s="63" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="K12" s="64"/>
       <c r="O12" s="2" t="str">
@@ -3300,9 +3246,11 @@
         <f t="shared" si="3"/>
         <v>IMG04</v>
       </c>
-      <c r="B13"/>
+      <c r="B13" t="s">
+        <v>205</v>
+      </c>
       <c r="C13" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso F6</v>
       </c>
       <c r="D13" s="63" t="s">
@@ -3327,24 +3275,20 @@
         <f ca="1">IF(OR($B13&lt;&gt;"",$J13&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
-      <c r="J13" s="63" t="s">
-        <v>199</v>
-      </c>
-      <c r="K13" s="64" t="s">
-        <v>200</v>
-      </c>
+      <c r="J13" s="63"/>
+      <c r="K13" s="64"/>
       <c r="O13" s="2" t="str">
         <f>'Definición técnica de imagenes'!A19</f>
         <v>F4</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="11" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="11" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG05</v>
       </c>
-      <c r="B14" s="62" t="s">
-        <v>202</v>
+      <c r="B14" s="62">
+        <v>329134130</v>
       </c>
       <c r="C14" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3373,7 +3317,7 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J14" s="63" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="K14" s="64"/>
       <c r="O14" s="2" t="str">
@@ -3381,13 +3325,13 @@
         <v>F6</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" ht="270" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG06</v>
       </c>
-      <c r="B15" s="62" t="s">
-        <v>193</v>
+      <c r="B15" s="79">
+        <v>352476497</v>
       </c>
       <c r="C15" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3416,7 +3360,7 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J15" s="63" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="K15" s="66"/>
       <c r="O15" s="2" t="str">
@@ -3424,13 +3368,13 @@
         <v>F6B</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="11" customFormat="1" ht="297" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG07</v>
       </c>
-      <c r="B16" s="62" t="s">
-        <v>196</v>
+      <c r="B16" s="78">
+        <v>54319891</v>
       </c>
       <c r="C16" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3459,7 +3403,7 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J16" s="63" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="K16" s="68"/>
       <c r="O16" s="2" t="str">
@@ -3472,7 +3416,9 @@
         <f t="shared" si="3"/>
         <v>IMG08</v>
       </c>
-      <c r="B17" s="62"/>
+      <c r="B17" s="62" t="s">
+        <v>201</v>
+      </c>
       <c r="C17" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F6</v>
@@ -3499,10 +3445,10 @@
         <f ca="1">IF(OR($B17&lt;&gt;"",$J17&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
-      <c r="J17" s="67" t="s">
-        <v>205</v>
-      </c>
-      <c r="K17" s="66"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="66" t="s">
+        <v>203</v>
+      </c>
       <c r="O17" s="2" t="str">
         <f>'Definición técnica de imagenes'!A27</f>
         <v>F7B</v>
@@ -3513,7 +3459,9 @@
         <f t="shared" si="3"/>
         <v>IMG09</v>
       </c>
-      <c r="B18" s="62"/>
+      <c r="B18" s="62" t="s">
+        <v>201</v>
+      </c>
       <c r="C18" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F6</v>
@@ -3540,10 +3488,10 @@
         <f ca="1">IF(OR($B18&lt;&gt;"",$J18&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
-      <c r="J18" s="67" t="s">
-        <v>206</v>
-      </c>
-      <c r="K18" s="66"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="66" t="s">
+        <v>204</v>
+      </c>
       <c r="O18" s="2" t="str">
         <f>'Definición técnica de imagenes'!A30</f>
         <v>F8</v>
@@ -3554,7 +3502,9 @@
         <f t="shared" ref="A19:A50" si="6">IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
         <v>IMG10</v>
       </c>
-      <c r="B19" s="62"/>
+      <c r="B19" s="78">
+        <v>2567351</v>
+      </c>
       <c r="C19" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F6</v>
@@ -3581,16 +3531,14 @@
         <f ca="1">IF(OR($B19&lt;&gt;"",$J19&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
-      <c r="J19" s="67" t="s">
-        <v>207</v>
-      </c>
+      <c r="J19" s="67"/>
       <c r="K19" s="68"/>
       <c r="O19" s="2" t="str">
         <f>'Definición técnica de imagenes'!A31</f>
         <v>F10</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="11" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" s="11" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="str">
         <f t="shared" si="6"/>
         <v>IMG11</v>
@@ -3623,7 +3571,7 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J20" s="64" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="K20" s="66"/>
       <c r="O20" s="2" t="str">
@@ -3664,7 +3612,7 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J21" s="64" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K21" s="66"/>
       <c r="O21" s="2" t="str">
@@ -3672,13 +3620,13 @@
         <v>F11</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="11" customFormat="1" ht="297" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="str">
         <f t="shared" si="6"/>
         <v>IMG13</v>
       </c>
-      <c r="B22" s="62" t="s">
-        <v>210</v>
+      <c r="B22" s="62">
+        <v>117359608</v>
       </c>
       <c r="C22" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3707,7 +3655,7 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J22" s="63" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="K22" s="69"/>
       <c r="O22" s="2" t="str">
@@ -3720,7 +3668,9 @@
         <f t="shared" si="6"/>
         <v>IMG14</v>
       </c>
-      <c r="B23" s="62"/>
+      <c r="B23" s="78">
+        <v>77819743</v>
+      </c>
       <c r="C23" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F6</v>
@@ -3748,7 +3698,7 @@
         <v/>
       </c>
       <c r="J23" s="64" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="K23" s="64"/>
       <c r="O23" s="2" t="str">
@@ -3756,36 +3706,44 @@
         <v>F13</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" s="11" customFormat="1" ht="248.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="B24" s="62"/>
+        <v>IMG15</v>
+      </c>
+      <c r="B24" s="62" t="s">
+        <v>201</v>
+      </c>
       <c r="C24" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D24" s="63"/>
-      <c r="E24" s="63"/>
+        <v>Recurso F6</v>
+      </c>
+      <c r="D24" s="63" t="s">
+        <v>192</v>
+      </c>
+      <c r="E24" s="63" t="s">
+        <v>155</v>
+      </c>
       <c r="F24" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" ca="1" si="4"/>
+        <v>MA_11_01_CO_REC50_IMG15n.jpg</v>
       </c>
       <c r="G24" s="13" t="str">
         <f ca="1">IF($F24&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E24,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>320 x 480 px</v>
       </c>
       <c r="H24" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>MA_11_01_CO_REC50_IMG15a.jpg</v>
       </c>
       <c r="I24" s="13" t="str">
         <f ca="1">IF(OR($B24&lt;&gt;"",$J24&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E24,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E24,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v/>
+        <v>800 x 458 px</v>
       </c>
       <c r="J24" s="63"/>
-      <c r="K24" s="65"/>
+      <c r="K24" s="65" t="s">
+        <v>202</v>
+      </c>
       <c r="O24" s="2" t="str">
         <f>'Definición técnica de imagenes'!A37</f>
         <v>F13B</v>
@@ -6400,7 +6358,7 @@
       <c r="K108" s="65"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="77H5Iqzv9dZcGmmBaf69JMJb19F7NL/TII5UwBSFOuUaqVrFbpC0VyStjTSM9GXqoLW1eBJcnDtnuP0mFWowpA==" saltValue="GBL6OckecvWR/Pgb/M/1sg==" spinCount="100000" sheet="1" scenarios="1" formatColumns="0" formatRows="0" selectLockedCells="1"/>
+  <sheetProtection formatColumns="0" formatRows="0" selectLockedCells="1"/>
   <mergeCells count="7">
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
@@ -6439,9 +6397,16 @@
       <formula1>$O$2:$O$27</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B11" r:id="rId1" display="http://www.shutterstock.com/pic-20092879/stock-vector-pi-number-on-many-digits-in-spiral.html?src=0I9hkwVXZTa01d19ktVamg-1-41"/>
+    <hyperlink ref="B12" r:id="rId2" display="http://www.shutterstock.com/pic-77507800/stock-photo-definition-of-golden-ratio-widely-used-in-mathematics-arts-architecture-and-design-white-chalk.html?src=S2hY6zlcnR_LSDDsrgq4Eg-1-31"/>
+    <hyperlink ref="B16" r:id="rId3" display="http://www.shutterstock.com/pic-54319891/stock-photo-a-man-with-a-big-calculator-which-shows-pi-number.html?src=0I9hkwVXZTa01d19ktVamg-1-24"/>
+    <hyperlink ref="B19" r:id="rId4" display="http://www.shutterstock.com/pic-2567351/stock-photo-concepto-del-n-mero-abstracto-n-mero-abstracto-delinfinito-del-e-del-n-mero-de-la-matem-ticas.html?src=pTdVBzaFhQ0StF08r9XsuQ-1-3"/>
+    <hyperlink ref="B23" r:id="rId5" display="http://www.shutterstock.com/pic-77819743/stock-photo-number-pi-portrait-of-young-scientist-calculating-pi-number.html?src=l-odcb3uveH8xWlZGK6jfA-3-41"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -6466,25 +6431,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="95"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="97"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="31"/>
-      <c r="C2" s="96" t="s">
+      <c r="C2" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="97"/>
-      <c r="E2" s="98"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="100"/>
       <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -6492,11 +6457,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="31"/>
-      <c r="C3" s="102" t="s">
+      <c r="C3" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="103"/>
-      <c r="E3" s="104"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="106"/>
       <c r="F3" s="32"/>
       <c r="H3" s="22" t="s">
         <v>18</v>
@@ -6547,11 +6512,11 @@
       <c r="C5" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="105" t="str">
+      <c r="D5" s="107" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="106"/>
+      <c r="E5" s="108"/>
       <c r="F5" s="32"/>
       <c r="H5" s="22" t="s">
         <v>22</v>
@@ -6596,12 +6561,12 @@
       <c r="C7" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="91" t="str">
+      <c r="D7" s="93" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="91"/>
-      <c r="F7" s="92"/>
+      <c r="E7" s="93"/>
+      <c r="F7" s="94"/>
       <c r="H7" s="22" t="s">
         <v>24</v>
       </c>
@@ -6695,14 +6660,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="95" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="94"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="94"/>
-      <c r="E13" s="94"/>
-      <c r="F13" s="95"/>
+      <c r="B13" s="96"/>
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="97"/>
       <c r="I13" s="22" t="s">
         <v>33</v>
       </c>
@@ -6735,12 +6700,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="31"/>
-      <c r="C15" s="96" t="s">
+      <c r="C15" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="97"/>
-      <c r="E15" s="97"/>
-      <c r="F15" s="98"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="99"/>
+      <c r="F15" s="100"/>
       <c r="J15" s="22">
         <v>12</v>
       </c>
@@ -6780,12 +6745,12 @@
       <c r="C17" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="99" t="str">
+      <c r="D17" s="101" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="100"/>
-      <c r="F17" s="101"/>
+      <c r="E17" s="102"/>
+      <c r="F17" s="103"/>
       <c r="J17" s="22">
         <v>14</v>
       </c>
@@ -6801,12 +6766,12 @@
       <c r="C18" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="91" t="str">
+      <c r="D18" s="93" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="91"/>
-      <c r="F18" s="92"/>
+      <c r="E18" s="93"/>
+      <c r="F18" s="94"/>
       <c r="J18" s="22">
         <v>15</v>
       </c>
@@ -7197,40 +7162,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="110" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="110" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="110" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="108" t="s">
+      <c r="D1" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="108" t="s">
+      <c r="F1" s="110" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="108" t="s">
+      <c r="G1" s="110" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="107" t="s">
+      <c r="H1" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="107"/>
+      <c r="I1" s="109"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="108"/>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
+      <c r="A2" s="110"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
       <c r="H2" s="39" t="s">
         <v>65</v>
       </c>

</xml_diff>